<commit_message>
Valida DNIs correctos y si no, corrige Excel
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="504">
   <si>
     <t>Nombre</t>
   </si>
@@ -1546,6 +1546,9 @@
   </si>
   <si>
     <t>3 1</t>
+  </si>
+  <si>
+    <t>prueba</t>
   </si>
 </sst>
 </file>
@@ -2045,7 +2048,7 @@
         <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>174</v>
+        <v>503</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>384</v>

</xml_diff>

<commit_message>
Desarrollo xml manager y genera ficheros xml
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="505">
   <si>
     <t>Nombre</t>
   </si>
@@ -1549,6 +1549,9 @@
   </si>
   <si>
     <t>prueba</t>
+  </si>
+  <si>
+    <t>09548416N</t>
   </si>
 </sst>
 </file>
@@ -2670,7 +2673,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>188</v>
+        <v>504</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -2758,7 +2761,7 @@
         <v>145</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>392</v>
@@ -3388,7 +3391,7 @@
         <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>394</v>
@@ -3564,7 +3567,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>397</v>
@@ -4503,7 +4506,7 @@
         <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>405</v>

</xml_diff>

<commit_message>
Corrigiendo errores FuncionDNI y adaptando practicaDos
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="503">
   <si>
     <t>Nombre</t>
   </si>
@@ -1546,12 +1546,6 @@
   </si>
   <si>
     <t>3 1</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>09548416N</t>
   </si>
 </sst>
 </file>
@@ -2051,7 +2045,7 @@
         <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>503</v>
+        <v>174</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>384</v>
@@ -2673,7 +2667,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>504</v>
+        <v>188</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -2761,7 +2755,7 @@
         <v>145</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>392</v>
@@ -3391,7 +3385,7 @@
         <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>394</v>
@@ -3567,7 +3561,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>397</v>
@@ -4506,7 +4500,7 @@
         <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>405</v>

</xml_diff>

<commit_message>
Corregido error de lectura contribuyentes guardados
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="504">
   <si>
     <t>Nombre</t>
   </si>
@@ -1546,6 +1546,9 @@
   </si>
   <si>
     <t>3 1</t>
+  </si>
+  <si>
+    <t>09548416N</t>
   </si>
 </sst>
 </file>
@@ -2667,7 +2670,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>188</v>
+        <v>503</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -2755,7 +2758,7 @@
         <v>145</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>392</v>
@@ -3385,7 +3388,7 @@
         <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>394</v>
@@ -3561,7 +3564,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>397</v>
@@ -4500,7 +4503,7 @@
         <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>405</v>

</xml_diff>

<commit_message>
Integrando todas las funciones creadas
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="672">
   <si>
     <t>Nombre</t>
   </si>
@@ -1549,6 +1549,510 @@
   </si>
   <si>
     <t>09548416N</t>
+  </si>
+  <si>
+    <t>DK7331645124473461205164</t>
+  </si>
+  <si>
+    <t>JMD00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES8265614874165615445616</t>
+  </si>
+  <si>
+    <t>RFM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>RO8832569523016220165156</t>
+  </si>
+  <si>
+    <t>ALM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DE7424561937521546497521</t>
+  </si>
+  <si>
+    <t>ALN00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>MC6436520125638451012515</t>
+  </si>
+  <si>
+    <t>RGO00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES0721584976902154655487</t>
+  </si>
+  <si>
+    <t>SDO00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>GR9420125003305201112544</t>
+  </si>
+  <si>
+    <t>VDO00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES2821651484690980008984</t>
+  </si>
+  <si>
+    <t>VBP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>FI5620960043043554600000</t>
+  </si>
+  <si>
+    <t>ABP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7921564975243245467995</t>
+  </si>
+  <si>
+    <t>MAP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>LT8032566221522587754554</t>
+  </si>
+  <si>
+    <t>ACP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>EE2023215465315456411515</t>
+  </si>
+  <si>
+    <t>LBP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>SM2125894363475485700145</t>
+  </si>
+  <si>
+    <t>LBR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9596431245118150005156</t>
+  </si>
+  <si>
+    <t>SBR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>AT6825030000114574745458</t>
+  </si>
+  <si>
+    <t>AGR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>IT8915953684811254695203</t>
+  </si>
+  <si>
+    <t>DGR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DK5800750184310702510000</t>
+  </si>
+  <si>
+    <t>CIS00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES5023455254943263234457</t>
+  </si>
+  <si>
+    <t>MQ00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>GR4920910936583000000000</t>
+  </si>
+  <si>
+    <t>BV00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES3720960043032159000000</t>
+  </si>
+  <si>
+    <t>PP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DE5512669681115112121210</t>
+  </si>
+  <si>
+    <t>PC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES2956187775315550000651</t>
+  </si>
+  <si>
+    <t>GMM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>CGM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>PT5764578946740051516490</t>
+  </si>
+  <si>
+    <t>GMM01@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>CSN00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>ALO00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>FR5623185484465641685100</t>
+  </si>
+  <si>
+    <t>GMM02@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DE5021508149175421346497</t>
+  </si>
+  <si>
+    <t>TCP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DE6721346154503164978451</t>
+  </si>
+  <si>
+    <t>CCP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7225187786311225455548</t>
+  </si>
+  <si>
+    <t>CAP00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>ELR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>DLR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>SPR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>GPR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>SAS00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>BFS00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>DFG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>GB9720910936583000000000</t>
+  </si>
+  <si>
+    <t>GMG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DE9301821135910205540000</t>
+  </si>
+  <si>
+    <t>MLG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>DE7822631245526916432102</t>
+  </si>
+  <si>
+    <t>IAG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES2120960043043075700000</t>
+  </si>
+  <si>
+    <t>IAG01@Agua2024.com</t>
+  </si>
+  <si>
+    <t>SM7325635478321002541225</t>
+  </si>
+  <si>
+    <t>GPG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES6832154697195423121000</t>
+  </si>
+  <si>
+    <t>RGG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>GB5520008521528775113366</t>
+  </si>
+  <si>
+    <t>AFG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>APM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>GB0836585214290025478551</t>
+  </si>
+  <si>
+    <t>GMM03@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>ALM01@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>LDM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>AD00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>LR00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>LC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>AFG01@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>DGG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>SOG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>PT3536952365020014425254</t>
+  </si>
+  <si>
+    <t>VVG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>VMG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>MBG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>CBG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>SDM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>EGM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>FI6132658012367712548745</t>
+  </si>
+  <si>
+    <t>GPM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>EAM00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>MG00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>JAC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>LT9321856333126985542360</t>
+  </si>
+  <si>
+    <t>BDC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>NGC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>MLC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>SE6832574512085411002255</t>
+  </si>
+  <si>
+    <t>MLC01@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>CFC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>CGC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>KSC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>AT8365645150865168448896</t>
+  </si>
+  <si>
+    <t>MHC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>26551681807651415636</t>
+  </si>
+  <si>
+    <t>IT3526551681807651415636</t>
+  </si>
+  <si>
+    <t>CLD00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>HU2399558741836555551120</t>
+  </si>
+  <si>
+    <t>MFD00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>51556584221251000254</t>
+  </si>
+  <si>
+    <t>IE6851556584221251000254</t>
+  </si>
+  <si>
+    <t>GMM04@Agua2024.com</t>
+  </si>
+  <si>
+    <t>62541122421110105611</t>
+  </si>
+  <si>
+    <t>LT9362541122421110105611</t>
+  </si>
+  <si>
+    <t>DMC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES6855065688761051056105</t>
+  </si>
+  <si>
+    <t>EBC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9712548521518742146695</t>
+  </si>
+  <si>
+    <t>MSC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9001826530120201560000</t>
+  </si>
+  <si>
+    <t>MDC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES9021651651812511133551</t>
+  </si>
+  <si>
+    <t>MFC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES6851651487910005118185</t>
+  </si>
+  <si>
+    <t>CDD00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>AT3122515651915640081000</t>
+  </si>
+  <si>
+    <t>HPD00@Agua2024.com</t>
   </si>
 </sst>
 </file>
@@ -2018,6 +2522,12 @@
       <c r="H2" s="3" t="s">
         <v>267</v>
       </c>
+      <c r="I2" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>505</v>
+      </c>
       <c r="K2" t="s" s="0">
         <v>264</v>
       </c>
@@ -2062,6 +2572,12 @@
       <c r="H3" s="3" t="s">
         <v>268</v>
       </c>
+      <c r="I3" t="s" s="0">
+        <v>506</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>507</v>
+      </c>
       <c r="K3" t="s" s="0">
         <v>264</v>
       </c>
@@ -2106,6 +2622,12 @@
       <c r="H4" s="3" t="s">
         <v>269</v>
       </c>
+      <c r="I4" t="s" s="0">
+        <v>508</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>509</v>
+      </c>
       <c r="K4" t="s" s="0">
         <v>264</v>
       </c>
@@ -2150,6 +2672,12 @@
       <c r="H5" s="3" t="s">
         <v>270</v>
       </c>
+      <c r="I5" t="s" s="0">
+        <v>510</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>511</v>
+      </c>
       <c r="K5" t="s" s="0">
         <v>264</v>
       </c>
@@ -2194,6 +2722,12 @@
       <c r="H6" s="3" t="s">
         <v>271</v>
       </c>
+      <c r="I6" t="s" s="0">
+        <v>512</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>513</v>
+      </c>
       <c r="K6" t="s" s="0">
         <v>264</v>
       </c>
@@ -2238,6 +2772,12 @@
       <c r="H7" s="3" t="s">
         <v>272</v>
       </c>
+      <c r="I7" t="s" s="0">
+        <v>514</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>515</v>
+      </c>
       <c r="K7" t="s" s="0">
         <v>264</v>
       </c>
@@ -2282,6 +2822,12 @@
       <c r="H8" s="3" t="s">
         <v>273</v>
       </c>
+      <c r="I8" t="s" s="0">
+        <v>516</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>517</v>
+      </c>
       <c r="K8" t="s" s="0">
         <v>264</v>
       </c>
@@ -2326,6 +2872,12 @@
       <c r="H9" s="3" t="s">
         <v>274</v>
       </c>
+      <c r="I9" t="s" s="0">
+        <v>518</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>519</v>
+      </c>
       <c r="K9" t="s" s="0">
         <v>264</v>
       </c>
@@ -2370,6 +2922,12 @@
       <c r="H10" s="3" t="s">
         <v>275</v>
       </c>
+      <c r="I10" t="s" s="0">
+        <v>520</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>521</v>
+      </c>
       <c r="K10" t="s" s="0">
         <v>264</v>
       </c>
@@ -2414,6 +2972,12 @@
       <c r="H11" s="3" t="s">
         <v>276</v>
       </c>
+      <c r="I11" t="s" s="0">
+        <v>522</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>523</v>
+      </c>
       <c r="K11" t="s" s="0">
         <v>264</v>
       </c>
@@ -2458,6 +3022,12 @@
       <c r="H12" s="3" t="s">
         <v>277</v>
       </c>
+      <c r="I12" t="s" s="0">
+        <v>524</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>525</v>
+      </c>
       <c r="K12" t="s" s="0">
         <v>264</v>
       </c>
@@ -2501,6 +3071,12 @@
       </c>
       <c r="H13" s="3" t="s">
         <v>278</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>526</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>527</v>
       </c>
       <c r="K13" t="s" s="0">
         <v>264</v>
@@ -2596,6 +3172,12 @@
       <c r="H16" s="3" t="s">
         <v>280</v>
       </c>
+      <c r="I16" t="s" s="0">
+        <v>528</v>
+      </c>
+      <c r="J16" t="s" s="0">
+        <v>529</v>
+      </c>
       <c r="K16" t="s" s="0">
         <v>264</v>
       </c>
@@ -2640,6 +3222,12 @@
       <c r="H17" s="3" t="s">
         <v>281</v>
       </c>
+      <c r="I17" t="s" s="0">
+        <v>530</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>531</v>
+      </c>
       <c r="K17" t="s" s="0">
         <v>264</v>
       </c>
@@ -2684,6 +3272,12 @@
       <c r="H18" s="3" t="s">
         <v>282</v>
       </c>
+      <c r="I18" t="s" s="0">
+        <v>532</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>533</v>
+      </c>
       <c r="K18" t="s" s="0">
         <v>264</v>
       </c>
@@ -2728,6 +3322,12 @@
       <c r="H19" s="3" t="s">
         <v>283</v>
       </c>
+      <c r="I19" t="s" s="0">
+        <v>534</v>
+      </c>
+      <c r="J19" t="s" s="0">
+        <v>535</v>
+      </c>
       <c r="K19" t="s" s="0">
         <v>264</v>
       </c>
@@ -2816,6 +3416,12 @@
       <c r="H21" s="3" t="s">
         <v>279</v>
       </c>
+      <c r="I21" t="s" s="0">
+        <v>536</v>
+      </c>
+      <c r="J21" t="s" s="0">
+        <v>537</v>
+      </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
       </c>
@@ -2857,6 +3463,12 @@
       <c r="H22" s="3" t="s">
         <v>285</v>
       </c>
+      <c r="I22" t="s" s="0">
+        <v>538</v>
+      </c>
+      <c r="J22" t="s" s="0">
+        <v>539</v>
+      </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
       </c>
@@ -2898,6 +3510,12 @@
       <c r="H23" s="3" t="s">
         <v>286</v>
       </c>
+      <c r="I23" t="s" s="0">
+        <v>540</v>
+      </c>
+      <c r="J23" t="s" s="0">
+        <v>541</v>
+      </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
       </c>
@@ -2939,6 +3557,12 @@
       <c r="H24" s="3" t="s">
         <v>287</v>
       </c>
+      <c r="I24" t="s" s="0">
+        <v>542</v>
+      </c>
+      <c r="J24" t="s" s="0">
+        <v>543</v>
+      </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
       </c>
@@ -2979,6 +3603,12 @@
       </c>
       <c r="H25" s="3" t="s">
         <v>288</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>544</v>
+      </c>
+      <c r="J25" t="s" s="0">
+        <v>545</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
@@ -3032,6 +3662,12 @@
       <c r="H27" s="3" t="s">
         <v>289</v>
       </c>
+      <c r="I27" t="s" s="0">
+        <v>546</v>
+      </c>
+      <c r="J27" t="s" s="0">
+        <v>547</v>
+      </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
       </c>
@@ -3076,6 +3712,12 @@
       <c r="H28" s="3" t="s">
         <v>290</v>
       </c>
+      <c r="I28" t="s" s="0">
+        <v>548</v>
+      </c>
+      <c r="J28" t="s" s="0">
+        <v>549</v>
+      </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
       </c>
@@ -3120,6 +3762,12 @@
       <c r="H29" s="3" t="s">
         <v>291</v>
       </c>
+      <c r="I29" t="s" s="0">
+        <v>550</v>
+      </c>
+      <c r="J29" t="s" s="0">
+        <v>551</v>
+      </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
       </c>
@@ -3164,6 +3812,12 @@
       <c r="H30" s="3" t="s">
         <v>292</v>
       </c>
+      <c r="I30" t="s" s="0">
+        <v>552</v>
+      </c>
+      <c r="J30" t="s" s="0">
+        <v>553</v>
+      </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
       </c>
@@ -3208,6 +3862,12 @@
       <c r="H31" s="3" t="s">
         <v>293</v>
       </c>
+      <c r="I31" t="s" s="0">
+        <v>554</v>
+      </c>
+      <c r="J31" t="s" s="0">
+        <v>555</v>
+      </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
       </c>
@@ -3251,6 +3911,12 @@
       </c>
       <c r="H32" s="3" t="s">
         <v>294</v>
+      </c>
+      <c r="I32" t="s" s="0">
+        <v>556</v>
+      </c>
+      <c r="J32" t="s" s="0">
+        <v>557</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -3314,6 +3980,12 @@
       <c r="H36" s="3" t="s">
         <v>295</v>
       </c>
+      <c r="I36" t="s" s="0">
+        <v>558</v>
+      </c>
+      <c r="J36" t="s" s="0">
+        <v>559</v>
+      </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
       </c>
@@ -3358,6 +4030,12 @@
       <c r="H37" s="3" t="s">
         <v>296</v>
       </c>
+      <c r="I37" t="s" s="0">
+        <v>560</v>
+      </c>
+      <c r="J37" t="s" s="0">
+        <v>561</v>
+      </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
       </c>
@@ -3402,6 +4080,12 @@
       <c r="H38" s="3" t="s">
         <v>297</v>
       </c>
+      <c r="I38" t="s" s="0">
+        <v>562</v>
+      </c>
+      <c r="J38" t="s" s="0">
+        <v>563</v>
+      </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
       </c>
@@ -3490,6 +4174,12 @@
       <c r="H40" s="3" t="s">
         <v>299</v>
       </c>
+      <c r="I40" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="J40" t="s" s="0">
+        <v>565</v>
+      </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
       </c>
@@ -3534,6 +4224,12 @@
       <c r="H41" s="3" t="s">
         <v>300</v>
       </c>
+      <c r="I41" t="s" s="0">
+        <v>566</v>
+      </c>
+      <c r="J41" t="s" s="0">
+        <v>567</v>
+      </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
       </c>
@@ -3622,6 +4318,12 @@
       <c r="H43" s="3" t="s">
         <v>302</v>
       </c>
+      <c r="I43" t="s" s="0">
+        <v>568</v>
+      </c>
+      <c r="J43" t="s" s="0">
+        <v>569</v>
+      </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
       </c>
@@ -3666,6 +4368,12 @@
       <c r="H44" s="3" t="s">
         <v>303</v>
       </c>
+      <c r="I44" t="s" s="0">
+        <v>570</v>
+      </c>
+      <c r="J44" t="s" s="0">
+        <v>571</v>
+      </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
       </c>
@@ -3710,6 +4418,12 @@
       <c r="H45" s="3" t="s">
         <v>304</v>
       </c>
+      <c r="I45" t="s" s="0">
+        <v>572</v>
+      </c>
+      <c r="J45" t="s" s="0">
+        <v>573</v>
+      </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
       </c>
@@ -3754,6 +4468,12 @@
       <c r="H46" s="3" t="s">
         <v>305</v>
       </c>
+      <c r="I46" t="s" s="0">
+        <v>574</v>
+      </c>
+      <c r="J46" t="s" s="0">
+        <v>575</v>
+      </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
       </c>
@@ -3798,6 +4518,12 @@
       <c r="H47" s="3" t="s">
         <v>306</v>
       </c>
+      <c r="I47" t="s" s="0">
+        <v>576</v>
+      </c>
+      <c r="J47" t="s" s="0">
+        <v>577</v>
+      </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
       </c>
@@ -3842,6 +4568,12 @@
       <c r="H48" s="3" t="s">
         <v>286</v>
       </c>
+      <c r="I48" t="s" s="0">
+        <v>578</v>
+      </c>
+      <c r="J48" t="s" s="0">
+        <v>579</v>
+      </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
       </c>
@@ -3886,6 +4618,12 @@
       <c r="H49" s="3" t="s">
         <v>307</v>
       </c>
+      <c r="I49" t="s" s="0">
+        <v>580</v>
+      </c>
+      <c r="J49" t="s" s="0">
+        <v>581</v>
+      </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
       </c>
@@ -3930,6 +4668,12 @@
       <c r="H50" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="I50" t="s" s="0">
+        <v>582</v>
+      </c>
+      <c r="J50" t="s" s="0">
+        <v>583</v>
+      </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
       </c>
@@ -3974,6 +4718,12 @@
       <c r="H51" s="3" t="s">
         <v>309</v>
       </c>
+      <c r="I51" t="s" s="0">
+        <v>584</v>
+      </c>
+      <c r="J51" t="s" s="0">
+        <v>585</v>
+      </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
       </c>
@@ -4018,6 +4768,12 @@
       <c r="H52" s="3" t="s">
         <v>310</v>
       </c>
+      <c r="I52" t="s" s="0">
+        <v>586</v>
+      </c>
+      <c r="J52" t="s" s="0">
+        <v>587</v>
+      </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
       </c>
@@ -4062,6 +4818,12 @@
       <c r="H53" s="3" t="s">
         <v>311</v>
       </c>
+      <c r="I53" t="s" s="0">
+        <v>588</v>
+      </c>
+      <c r="J53" t="s" s="0">
+        <v>589</v>
+      </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
       </c>
@@ -4149,6 +4911,12 @@
       </c>
       <c r="H55" s="3" t="s">
         <v>313</v>
+      </c>
+      <c r="I55" t="s" s="0">
+        <v>590</v>
+      </c>
+      <c r="J55" t="s" s="0">
+        <v>591</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -4218,6 +4986,12 @@
       <c r="H60" s="3" t="s">
         <v>314</v>
       </c>
+      <c r="I60" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="J60" t="s" s="0">
+        <v>593</v>
+      </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
       </c>
@@ -4262,6 +5036,12 @@
       <c r="H61" s="3" t="s">
         <v>315</v>
       </c>
+      <c r="I61" t="s" s="0">
+        <v>594</v>
+      </c>
+      <c r="J61" t="s" s="0">
+        <v>595</v>
+      </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
       </c>
@@ -4306,6 +5086,12 @@
       <c r="H62" s="3" t="s">
         <v>316</v>
       </c>
+      <c r="I62" t="s" s="0">
+        <v>596</v>
+      </c>
+      <c r="J62" t="s" s="0">
+        <v>597</v>
+      </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
       </c>
@@ -4350,6 +5136,12 @@
       <c r="H63" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="I63" t="s" s="0">
+        <v>598</v>
+      </c>
+      <c r="J63" t="s" s="0">
+        <v>599</v>
+      </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
       </c>
@@ -4391,6 +5183,12 @@
       <c r="H64" s="3" t="s">
         <v>318</v>
       </c>
+      <c r="I64" t="s" s="0">
+        <v>600</v>
+      </c>
+      <c r="J64" t="s" s="0">
+        <v>601</v>
+      </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
       </c>
@@ -4432,6 +5230,12 @@
       <c r="H65" s="3" t="s">
         <v>319</v>
       </c>
+      <c r="I65" t="s" s="0">
+        <v>602</v>
+      </c>
+      <c r="J65" t="s" s="0">
+        <v>603</v>
+      </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
       </c>
@@ -4473,6 +5277,12 @@
       <c r="H66" s="3" t="s">
         <v>320</v>
       </c>
+      <c r="I66" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="J66" t="s" s="0">
+        <v>605</v>
+      </c>
       <c r="K66" t="s" s="0">
         <v>264</v>
       </c>
@@ -4561,6 +5371,12 @@
       <c r="H68" s="3" t="s">
         <v>322</v>
       </c>
+      <c r="I68" t="s" s="0">
+        <v>606</v>
+      </c>
+      <c r="J68" t="s" s="0">
+        <v>607</v>
+      </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
       </c>
@@ -4605,6 +5421,12 @@
       <c r="H69" s="3" t="s">
         <v>323</v>
       </c>
+      <c r="I69" t="s" s="0">
+        <v>608</v>
+      </c>
+      <c r="J69" t="s" s="0">
+        <v>609</v>
+      </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
       </c>
@@ -4693,6 +5515,12 @@
       <c r="H71" s="3" t="s">
         <v>314</v>
       </c>
+      <c r="I71" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="J71" t="s" s="0">
+        <v>610</v>
+      </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
       </c>
@@ -4737,6 +5565,12 @@
       <c r="H72" s="3" t="s">
         <v>325</v>
       </c>
+      <c r="I72" t="s" s="0">
+        <v>611</v>
+      </c>
+      <c r="J72" t="s" s="0">
+        <v>612</v>
+      </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
       </c>
@@ -4781,6 +5615,12 @@
       <c r="H73" s="3" t="s">
         <v>326</v>
       </c>
+      <c r="I73" t="s" s="0">
+        <v>613</v>
+      </c>
+      <c r="J73" t="s" s="0">
+        <v>614</v>
+      </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
       </c>
@@ -4825,6 +5665,12 @@
       <c r="H74" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="I74" t="s" s="0">
+        <v>615</v>
+      </c>
+      <c r="J74" t="s" s="0">
+        <v>616</v>
+      </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
       </c>
@@ -4868,6 +5714,12 @@
       </c>
       <c r="H75" s="3" t="s">
         <v>328</v>
+      </c>
+      <c r="I75" t="s" s="0">
+        <v>617</v>
+      </c>
+      <c r="J75" t="s" s="0">
+        <v>618</v>
       </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
@@ -5007,6 +5859,12 @@
       <c r="H79" s="3" t="s">
         <v>331</v>
       </c>
+      <c r="I79" t="s" s="0">
+        <v>619</v>
+      </c>
+      <c r="J79" t="s" s="0">
+        <v>620</v>
+      </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
       </c>
@@ -5049,7 +5907,13 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>332</v>
+        <v>621</v>
+      </c>
+      <c r="I80" t="s" s="0">
+        <v>622</v>
+      </c>
+      <c r="J80" t="s" s="0">
+        <v>623</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
@@ -5095,6 +5959,12 @@
       <c r="H81" s="3" t="s">
         <v>333</v>
       </c>
+      <c r="I81" t="s" s="0">
+        <v>624</v>
+      </c>
+      <c r="J81" t="s" s="0">
+        <v>625</v>
+      </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
       </c>
@@ -5139,6 +6009,12 @@
       <c r="H82" s="3" t="s">
         <v>334</v>
       </c>
+      <c r="I82" t="s" s="0">
+        <v>626</v>
+      </c>
+      <c r="J82" t="s" s="0">
+        <v>627</v>
+      </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
       </c>
@@ -5223,6 +6099,12 @@
       </c>
       <c r="H84" s="3" t="s">
         <v>336</v>
+      </c>
+      <c r="I84" t="s" s="0">
+        <v>628</v>
+      </c>
+      <c r="J84" t="s" s="0">
+        <v>629</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -5274,6 +6156,12 @@
       <c r="H86" s="3" t="s">
         <v>337</v>
       </c>
+      <c r="I86" t="s" s="0">
+        <v>630</v>
+      </c>
+      <c r="J86" t="s" s="0">
+        <v>631</v>
+      </c>
       <c r="K86" t="s" s="0">
         <v>264</v>
       </c>
@@ -5318,6 +6206,12 @@
       <c r="H87" s="3" t="s">
         <v>338</v>
       </c>
+      <c r="I87" t="s" s="0">
+        <v>632</v>
+      </c>
+      <c r="J87" t="s" s="0">
+        <v>633</v>
+      </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
       </c>
@@ -5362,6 +6256,12 @@
       <c r="H88" s="3" t="s">
         <v>339</v>
       </c>
+      <c r="I88" t="s" s="0">
+        <v>634</v>
+      </c>
+      <c r="J88" t="s" s="0">
+        <v>635</v>
+      </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
       </c>
@@ -5406,6 +6306,12 @@
       <c r="H89" s="3" t="s">
         <v>340</v>
       </c>
+      <c r="I89" t="s" s="0">
+        <v>636</v>
+      </c>
+      <c r="J89" t="s" s="0">
+        <v>637</v>
+      </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
       </c>
@@ -5491,6 +6397,12 @@
       <c r="H91" s="3" t="s">
         <v>342</v>
       </c>
+      <c r="I91" t="s" s="0">
+        <v>638</v>
+      </c>
+      <c r="J91" t="s" s="0">
+        <v>639</v>
+      </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
       </c>
@@ -5535,6 +6447,12 @@
       <c r="H92" s="3" t="s">
         <v>343</v>
       </c>
+      <c r="I92" t="s" s="0">
+        <v>640</v>
+      </c>
+      <c r="J92" t="s" s="0">
+        <v>641</v>
+      </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
       </c>
@@ -5579,6 +6497,12 @@
       <c r="H93" s="3" t="s">
         <v>344</v>
       </c>
+      <c r="I93" t="s" s="0">
+        <v>642</v>
+      </c>
+      <c r="J93" t="s" s="0">
+        <v>643</v>
+      </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
       </c>
@@ -5664,6 +6588,12 @@
       </c>
       <c r="H95" s="3" t="s">
         <v>346</v>
+      </c>
+      <c r="I95" t="s" s="0">
+        <v>644</v>
+      </c>
+      <c r="J95" t="s" s="0">
+        <v>645</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -5743,7 +6673,13 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>347</v>
+        <v>646</v>
+      </c>
+      <c r="I102" t="s" s="0">
+        <v>647</v>
+      </c>
+      <c r="J102" t="s" s="0">
+        <v>648</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -5787,7 +6723,13 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>348</v>
+        <v>649</v>
+      </c>
+      <c r="I103" t="s" s="0">
+        <v>650</v>
+      </c>
+      <c r="J103" t="s" s="0">
+        <v>651</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
@@ -5833,6 +6775,12 @@
       <c r="H104" s="3" t="s">
         <v>349</v>
       </c>
+      <c r="I104" t="s" s="0">
+        <v>652</v>
+      </c>
+      <c r="J104" t="s" s="0">
+        <v>653</v>
+      </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
       </c>
@@ -5919,7 +6867,13 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>351</v>
+        <v>654</v>
+      </c>
+      <c r="I106" t="s" s="0">
+        <v>655</v>
+      </c>
+      <c r="J106" t="s" s="0">
+        <v>656</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
@@ -6127,7 +7081,13 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>353</v>
+        <v>657</v>
+      </c>
+      <c r="I128" t="s" s="0">
+        <v>658</v>
+      </c>
+      <c r="J128" t="s" s="0">
+        <v>659</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -6173,6 +7133,12 @@
       <c r="H129" s="3" t="s">
         <v>354</v>
       </c>
+      <c r="I129" t="s" s="0">
+        <v>660</v>
+      </c>
+      <c r="J129" t="s" s="0">
+        <v>661</v>
+      </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
       </c>
@@ -6261,6 +7227,12 @@
       <c r="H131" s="3" t="s">
         <v>356</v>
       </c>
+      <c r="I131" t="s" s="0">
+        <v>662</v>
+      </c>
+      <c r="J131" t="s" s="0">
+        <v>663</v>
+      </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
       </c>
@@ -6305,6 +7277,12 @@
       <c r="H132" s="3" t="s">
         <v>357</v>
       </c>
+      <c r="I132" t="s" s="0">
+        <v>664</v>
+      </c>
+      <c r="J132" t="s" s="0">
+        <v>665</v>
+      </c>
       <c r="K132" t="s" s="0">
         <v>264</v>
       </c>
@@ -6349,6 +7327,12 @@
       <c r="H133" s="3" t="s">
         <v>358</v>
       </c>
+      <c r="I133" t="s" s="0">
+        <v>666</v>
+      </c>
+      <c r="J133" t="s" s="0">
+        <v>667</v>
+      </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
       </c>
@@ -6393,6 +7377,12 @@
       <c r="H134" s="3" t="s">
         <v>359</v>
       </c>
+      <c r="I134" t="s" s="0">
+        <v>668</v>
+      </c>
+      <c r="J134" t="s" s="0">
+        <v>669</v>
+      </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
       </c>
@@ -6478,6 +7468,12 @@
       </c>
       <c r="H136" s="3" t="s">
         <v>361</v>
+      </c>
+      <c r="I136" t="s" s="0">
+        <v>670</v>
+      </c>
+      <c r="J136" t="s" s="0">
+        <v>671</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>

</xml_diff>

<commit_message>
Tratamiento de fechas y correccion de errores
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="686">
   <si>
     <t>Nombre</t>
   </si>
@@ -1647,6 +1647,12 @@
     <t>DGR00@Agua2024.com</t>
   </si>
   <si>
+    <t>ES9020960043023096200000</t>
+  </si>
+  <si>
+    <t>PGS00@Agua2024.com</t>
+  </si>
+  <si>
     <t>DK5800750184310702510000</t>
   </si>
   <si>
@@ -1731,6 +1737,12 @@
     <t>CAP00@Agua2024.com</t>
   </si>
   <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>SFP00@Agua2024.com</t>
+  </si>
+  <si>
     <t>ES2396536214865214585214</t>
   </si>
   <si>
@@ -1743,6 +1755,12 @@
     <t>DLR00@Agua2024.com</t>
   </si>
   <si>
+    <t>FI5024587946032003165464</t>
+  </si>
+  <si>
+    <t>HAR00@Agua2024.com</t>
+  </si>
+  <si>
     <t>ES5020960043073071400000</t>
   </si>
   <si>
@@ -1851,10 +1869,10 @@
     <t>LR00@Agua2024.com</t>
   </si>
   <si>
-    <t>ES7920960031442124800000</t>
-  </si>
-  <si>
-    <t>LC00@Agua2024.com</t>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>SBG00@Agua2024.com</t>
   </si>
   <si>
     <t>ES1933218885441445121022</t>
@@ -1869,6 +1887,12 @@
     <t>DGG00@Agua2024.com</t>
   </si>
   <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>ROG00@Agua2024.com</t>
+  </si>
+  <si>
     <t>SOG00@Agua2024.com</t>
   </si>
   <si>
@@ -1896,6 +1920,12 @@
     <t>CBG00@Agua2024.com</t>
   </si>
   <si>
+    <t>LU0932628484504115151115</t>
+  </si>
+  <si>
+    <t>MSH00@Agua2024.com</t>
+  </si>
+  <si>
     <t>ES8163516541828944000984</t>
   </si>
   <si>
@@ -1929,12 +1959,6 @@
     <t>MG00@Agua2024.com</t>
   </si>
   <si>
-    <t>ES7395485212315484010000</t>
-  </si>
-  <si>
-    <t>JAC00@Agua2024.com</t>
-  </si>
-  <si>
     <t>LT9321856333126985542360</t>
   </si>
   <si>
@@ -1953,6 +1977,12 @@
     <t>MLC00@Agua2024.com</t>
   </si>
   <si>
+    <t>SM4423221158252545471411</t>
+  </si>
+  <si>
+    <t>MH00@Agua2024.com</t>
+  </si>
+  <si>
     <t>SE6832574512085411002255</t>
   </si>
   <si>
@@ -2010,6 +2040,12 @@
     <t>GMM04@Agua2024.com</t>
   </si>
   <si>
+    <t>DK9032541112811220000588</t>
+  </si>
+  <si>
+    <t>IVC00@Agua2024.com</t>
+  </si>
+  <si>
     <t>62541122421110105611</t>
   </si>
   <si>
@@ -2023,6 +2059,12 @@
   </si>
   <si>
     <t>EBC00@Agua2024.com</t>
+  </si>
+  <si>
+    <t>ES7426221011628048788896</t>
+  </si>
+  <si>
+    <t>NBC00@Agua2024.com</t>
   </si>
   <si>
     <t>ES9712548521518742146695</t>
@@ -3372,6 +3414,12 @@
       <c r="H20" s="3" t="s">
         <v>284</v>
       </c>
+      <c r="I20" t="s" s="0">
+        <v>536</v>
+      </c>
+      <c r="J20" t="s" s="0">
+        <v>537</v>
+      </c>
       <c r="K20" t="s" s="0">
         <v>264</v>
       </c>
@@ -3417,10 +3465,10 @@
         <v>279</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="J21" t="s" s="0">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
@@ -3464,10 +3512,10 @@
         <v>285</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="J22" t="s" s="0">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
@@ -3511,10 +3559,10 @@
         <v>286</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="J23" t="s" s="0">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
@@ -3558,10 +3606,10 @@
         <v>287</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="J24" t="s" s="0">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
@@ -3605,10 +3653,10 @@
         <v>288</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="J25" t="s" s="0">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
@@ -3663,10 +3711,10 @@
         <v>289</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="J27" t="s" s="0">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
@@ -3713,10 +3761,10 @@
         <v>290</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="J28" t="s" s="0">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
@@ -3763,10 +3811,10 @@
         <v>291</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="J29" t="s" s="0">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
@@ -3813,10 +3861,10 @@
         <v>292</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="J30" t="s" s="0">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
@@ -3863,10 +3911,10 @@
         <v>293</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="J31" t="s" s="0">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
@@ -3913,10 +3961,10 @@
         <v>294</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -3981,10 +4029,10 @@
         <v>295</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="J36" t="s" s="0">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
@@ -4031,10 +4079,10 @@
         <v>296</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="J37" t="s" s="0">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
@@ -4081,10 +4129,10 @@
         <v>297</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="J38" t="s" s="0">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
@@ -4130,6 +4178,12 @@
       <c r="H39" s="3" t="s">
         <v>298</v>
       </c>
+      <c r="I39" t="s" s="0">
+        <v>566</v>
+      </c>
+      <c r="J39" t="s" s="0">
+        <v>567</v>
+      </c>
       <c r="K39" t="s" s="0">
         <v>264</v>
       </c>
@@ -4175,10 +4229,10 @@
         <v>299</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="J40" t="s" s="0">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
@@ -4225,10 +4279,10 @@
         <v>300</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="J41" t="s" s="0">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
@@ -4274,6 +4328,12 @@
       <c r="H42" s="3" t="s">
         <v>301</v>
       </c>
+      <c r="I42" t="s" s="0">
+        <v>572</v>
+      </c>
+      <c r="J42" t="s" s="0">
+        <v>573</v>
+      </c>
       <c r="K42" t="s" s="0">
         <v>264</v>
       </c>
@@ -4319,10 +4379,10 @@
         <v>302</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="J43" t="s" s="0">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
@@ -4369,10 +4429,10 @@
         <v>303</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="J44" t="s" s="0">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
@@ -4419,10 +4479,10 @@
         <v>304</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="J45" t="s" s="0">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
@@ -4469,10 +4529,10 @@
         <v>305</v>
       </c>
       <c r="I46" t="s" s="0">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="J46" t="s" s="0">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
@@ -4519,10 +4579,10 @@
         <v>306</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="J47" t="s" s="0">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
@@ -4569,10 +4629,10 @@
         <v>286</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="J48" t="s" s="0">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
@@ -4619,10 +4679,10 @@
         <v>307</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="J49" t="s" s="0">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
@@ -4669,10 +4729,10 @@
         <v>308</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="J50" t="s" s="0">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
@@ -4719,10 +4779,10 @@
         <v>309</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="J51" t="s" s="0">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
@@ -4769,10 +4829,10 @@
         <v>310</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="J52" t="s" s="0">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
@@ -4819,10 +4879,10 @@
         <v>311</v>
       </c>
       <c r="I53" t="s" s="0">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="J53" t="s" s="0">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
@@ -4913,10 +4973,10 @@
         <v>313</v>
       </c>
       <c r="I55" t="s" s="0">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c r="J55" t="s" s="0">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -4987,10 +5047,10 @@
         <v>314</v>
       </c>
       <c r="I60" t="s" s="0">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="J60" t="s" s="0">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
@@ -5037,10 +5097,10 @@
         <v>315</v>
       </c>
       <c r="I61" t="s" s="0">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="J61" t="s" s="0">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
@@ -5087,10 +5147,10 @@
         <v>316</v>
       </c>
       <c r="I62" t="s" s="0">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="J62" t="s" s="0">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
@@ -5137,10 +5197,10 @@
         <v>317</v>
       </c>
       <c r="I63" t="s" s="0">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c r="J63" t="s" s="0">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
@@ -5184,10 +5244,10 @@
         <v>318</v>
       </c>
       <c r="I64" t="s" s="0">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="J64" t="s" s="0">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
@@ -5231,10 +5291,10 @@
         <v>319</v>
       </c>
       <c r="I65" t="s" s="0">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="J65" t="s" s="0">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
@@ -5277,12 +5337,6 @@
       <c r="H66" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="I66" t="s" s="0">
-        <v>604</v>
-      </c>
-      <c r="J66" t="s" s="0">
-        <v>605</v>
-      </c>
       <c r="K66" t="s" s="0">
         <v>264</v>
       </c>
@@ -5327,6 +5381,12 @@
       <c r="H67" s="3" t="s">
         <v>321</v>
       </c>
+      <c r="I67" t="s" s="0">
+        <v>610</v>
+      </c>
+      <c r="J67" t="s" s="0">
+        <v>611</v>
+      </c>
       <c r="K67" t="s" s="0">
         <v>264</v>
       </c>
@@ -5372,10 +5432,10 @@
         <v>322</v>
       </c>
       <c r="I68" t="s" s="0">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="J68" t="s" s="0">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
@@ -5422,10 +5482,10 @@
         <v>323</v>
       </c>
       <c r="I69" t="s" s="0">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="J69" t="s" s="0">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
@@ -5471,6 +5531,12 @@
       <c r="H70" s="3" t="s">
         <v>324</v>
       </c>
+      <c r="I70" t="s" s="0">
+        <v>616</v>
+      </c>
+      <c r="J70" t="s" s="0">
+        <v>617</v>
+      </c>
       <c r="K70" t="s" s="0">
         <v>264</v>
       </c>
@@ -5516,10 +5582,10 @@
         <v>314</v>
       </c>
       <c r="I71" t="s" s="0">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="J71" t="s" s="0">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
@@ -5566,10 +5632,10 @@
         <v>325</v>
       </c>
       <c r="I72" t="s" s="0">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="J72" t="s" s="0">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
@@ -5616,10 +5682,10 @@
         <v>326</v>
       </c>
       <c r="I73" t="s" s="0">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="J73" t="s" s="0">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
@@ -5666,10 +5732,10 @@
         <v>327</v>
       </c>
       <c r="I74" t="s" s="0">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="J74" t="s" s="0">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
@@ -5716,10 +5782,10 @@
         <v>328</v>
       </c>
       <c r="I75" t="s" s="0">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="J75" t="s" s="0">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
@@ -5764,6 +5830,12 @@
       </c>
       <c r="H76" s="3" t="s">
         <v>329</v>
+      </c>
+      <c r="I76" t="s" s="0">
+        <v>627</v>
+      </c>
+      <c r="J76" t="s" s="0">
+        <v>628</v>
       </c>
       <c r="K76" t="s" s="0">
         <v>264</v>
@@ -5860,10 +5932,10 @@
         <v>331</v>
       </c>
       <c r="I79" t="s" s="0">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="J79" t="s" s="0">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
@@ -5907,13 +5979,13 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>621</v>
+        <v>631</v>
       </c>
       <c r="I80" t="s" s="0">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="J80" t="s" s="0">
-        <v>623</v>
+        <v>633</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
@@ -5960,10 +6032,10 @@
         <v>333</v>
       </c>
       <c r="I81" t="s" s="0">
-        <v>624</v>
+        <v>634</v>
       </c>
       <c r="J81" t="s" s="0">
-        <v>625</v>
+        <v>635</v>
       </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
@@ -6010,10 +6082,10 @@
         <v>334</v>
       </c>
       <c r="I82" t="s" s="0">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="J82" t="s" s="0">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
@@ -6101,10 +6173,10 @@
         <v>336</v>
       </c>
       <c r="I84" t="s" s="0">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="J84" t="s" s="0">
-        <v>629</v>
+        <v>639</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -6156,12 +6228,6 @@
       <c r="H86" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="I86" t="s" s="0">
-        <v>630</v>
-      </c>
-      <c r="J86" t="s" s="0">
-        <v>631</v>
-      </c>
       <c r="K86" t="s" s="0">
         <v>264</v>
       </c>
@@ -6207,10 +6273,10 @@
         <v>338</v>
       </c>
       <c r="I87" t="s" s="0">
-        <v>632</v>
+        <v>640</v>
       </c>
       <c r="J87" t="s" s="0">
-        <v>633</v>
+        <v>641</v>
       </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
@@ -6257,10 +6323,10 @@
         <v>339</v>
       </c>
       <c r="I88" t="s" s="0">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="J88" t="s" s="0">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
@@ -6307,10 +6373,10 @@
         <v>340</v>
       </c>
       <c r="I89" t="s" s="0">
-        <v>636</v>
+        <v>644</v>
       </c>
       <c r="J89" t="s" s="0">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
@@ -6353,6 +6419,12 @@
       <c r="H90" s="3" t="s">
         <v>341</v>
       </c>
+      <c r="I90" t="s" s="0">
+        <v>646</v>
+      </c>
+      <c r="J90" t="s" s="0">
+        <v>647</v>
+      </c>
       <c r="K90" t="s" s="0">
         <v>264</v>
       </c>
@@ -6398,10 +6470,10 @@
         <v>342</v>
       </c>
       <c r="I91" t="s" s="0">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="J91" t="s" s="0">
-        <v>639</v>
+        <v>649</v>
       </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
@@ -6448,10 +6520,10 @@
         <v>343</v>
       </c>
       <c r="I92" t="s" s="0">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="J92" t="s" s="0">
-        <v>641</v>
+        <v>651</v>
       </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
@@ -6498,10 +6570,10 @@
         <v>344</v>
       </c>
       <c r="I93" t="s" s="0">
-        <v>642</v>
+        <v>652</v>
       </c>
       <c r="J93" t="s" s="0">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
@@ -6590,10 +6662,10 @@
         <v>346</v>
       </c>
       <c r="I95" t="s" s="0">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="J95" t="s" s="0">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -6673,13 +6745,13 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>646</v>
+        <v>656</v>
       </c>
       <c r="I102" t="s" s="0">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="J102" t="s" s="0">
-        <v>648</v>
+        <v>658</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -6723,13 +6795,13 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="I103" t="s" s="0">
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="J103" t="s" s="0">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
@@ -6776,10 +6848,10 @@
         <v>349</v>
       </c>
       <c r="I104" t="s" s="0">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="J104" t="s" s="0">
-        <v>653</v>
+        <v>663</v>
       </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
@@ -6867,13 +6939,13 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="I106" t="s" s="0">
-        <v>655</v>
+        <v>665</v>
       </c>
       <c r="J106" t="s" s="0">
-        <v>656</v>
+        <v>666</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
@@ -7039,6 +7111,12 @@
       <c r="H127" s="3" t="s">
         <v>352</v>
       </c>
+      <c r="I127" t="s" s="0">
+        <v>667</v>
+      </c>
+      <c r="J127" t="s" s="0">
+        <v>668</v>
+      </c>
       <c r="K127" t="s" s="0">
         <v>264</v>
       </c>
@@ -7081,13 +7159,13 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>657</v>
+        <v>669</v>
       </c>
       <c r="I128" t="s" s="0">
-        <v>658</v>
+        <v>670</v>
       </c>
       <c r="J128" t="s" s="0">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -7134,10 +7212,10 @@
         <v>354</v>
       </c>
       <c r="I129" t="s" s="0">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="J129" t="s" s="0">
-        <v>661</v>
+        <v>673</v>
       </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
@@ -7183,6 +7261,12 @@
       <c r="H130" s="3" t="s">
         <v>355</v>
       </c>
+      <c r="I130" t="s" s="0">
+        <v>674</v>
+      </c>
+      <c r="J130" t="s" s="0">
+        <v>675</v>
+      </c>
       <c r="K130" t="s" s="0">
         <v>264</v>
       </c>
@@ -7228,10 +7312,10 @@
         <v>356</v>
       </c>
       <c r="I131" t="s" s="0">
-        <v>662</v>
+        <v>676</v>
       </c>
       <c r="J131" t="s" s="0">
-        <v>663</v>
+        <v>677</v>
       </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
@@ -7278,10 +7362,10 @@
         <v>357</v>
       </c>
       <c r="I132" t="s" s="0">
-        <v>664</v>
+        <v>678</v>
       </c>
       <c r="J132" t="s" s="0">
-        <v>665</v>
+        <v>679</v>
       </c>
       <c r="K132" t="s" s="0">
         <v>264</v>
@@ -7328,10 +7412,10 @@
         <v>358</v>
       </c>
       <c r="I133" t="s" s="0">
-        <v>666</v>
+        <v>680</v>
       </c>
       <c r="J133" t="s" s="0">
-        <v>667</v>
+        <v>681</v>
       </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
@@ -7378,10 +7462,10 @@
         <v>359</v>
       </c>
       <c r="I134" t="s" s="0">
-        <v>668</v>
+        <v>682</v>
       </c>
       <c r="J134" t="s" s="0">
-        <v>669</v>
+        <v>683</v>
       </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
@@ -7470,10 +7554,10 @@
         <v>361</v>
       </c>
       <c r="I136" t="s" s="0">
-        <v>670</v>
+        <v>684</v>
       </c>
       <c r="J136" t="s" s="0">
-        <v>671</v>
+        <v>685</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>

</xml_diff>

<commit_message>
Implementando practica 3 sin terminar
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAguaTrasEjecucion.xlsx
+++ b/src/resources/SistemasAguaTrasEjecucion.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="503">
   <si>
     <t>Nombre</t>
   </si>
@@ -1546,555 +1546,6 @@
   </si>
   <si>
     <t>3 1</t>
-  </si>
-  <si>
-    <t>09548416N</t>
-  </si>
-  <si>
-    <t>DK7331645124473461205164</t>
-  </si>
-  <si>
-    <t>JMD00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES8265614874165615445616</t>
-  </si>
-  <si>
-    <t>RFM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>RO8832569523016220165156</t>
-  </si>
-  <si>
-    <t>ALM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DE7424561937521546497521</t>
-  </si>
-  <si>
-    <t>ALN00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>MC6436520125638451012515</t>
-  </si>
-  <si>
-    <t>RGO00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES0721584976902154655487</t>
-  </si>
-  <si>
-    <t>SDO00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>GR9420125003305201112544</t>
-  </si>
-  <si>
-    <t>VDO00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES2821651484690980008984</t>
-  </si>
-  <si>
-    <t>VBP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>FI5620960043043554600000</t>
-  </si>
-  <si>
-    <t>ABP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7921564975243245467995</t>
-  </si>
-  <si>
-    <t>MAP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>LT8032566221522587754554</t>
-  </si>
-  <si>
-    <t>ACP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>EE2023215465315456411515</t>
-  </si>
-  <si>
-    <t>LBP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>SM2125894363475485700145</t>
-  </si>
-  <si>
-    <t>LBR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9596431245118150005156</t>
-  </si>
-  <si>
-    <t>SBR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>AT6825030000114574745458</t>
-  </si>
-  <si>
-    <t>AGR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>IT8915953684811254695203</t>
-  </si>
-  <si>
-    <t>DGR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9020960043023096200000</t>
-  </si>
-  <si>
-    <t>PGS00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DK5800750184310702510000</t>
-  </si>
-  <si>
-    <t>CIS00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES5023455254943263234457</t>
-  </si>
-  <si>
-    <t>MQ00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>GR4920910936583000000000</t>
-  </si>
-  <si>
-    <t>BV00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES3720960043032159000000</t>
-  </si>
-  <si>
-    <t>PP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DE5512669681115112121210</t>
-  </si>
-  <si>
-    <t>PC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES2956187775315550000651</t>
-  </si>
-  <si>
-    <t>GMM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES0425516848021156151054</t>
-  </si>
-  <si>
-    <t>CGM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>PT5764578946740051516490</t>
-  </si>
-  <si>
-    <t>GMM01@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES4534698752714600549403</t>
-  </si>
-  <si>
-    <t>CSN00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES2766649444162310000255</t>
-  </si>
-  <si>
-    <t>ALO00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>FR5623185484465641685100</t>
-  </si>
-  <si>
-    <t>GMM02@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DE5021508149175421346497</t>
-  </si>
-  <si>
-    <t>TCP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DE6721346154503164978451</t>
-  </si>
-  <si>
-    <t>CCP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7225187786311225455548</t>
-  </si>
-  <si>
-    <t>CAP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES4723164897642213030615</t>
-  </si>
-  <si>
-    <t>SFP00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES2396536214865214585214</t>
-  </si>
-  <si>
-    <t>ELR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES6885461325251978750005</t>
-  </si>
-  <si>
-    <t>DLR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>FI5024587946032003165464</t>
-  </si>
-  <si>
-    <t>HAR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES5020960043073071400000</t>
-  </si>
-  <si>
-    <t>SPR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES8220960043042158800000</t>
-  </si>
-  <si>
-    <t>GPR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7521654587985156484454</t>
-  </si>
-  <si>
-    <t>SAS00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES3251651681961210656510</t>
-  </si>
-  <si>
-    <t>BFS00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES5566552211148855332200</t>
-  </si>
-  <si>
-    <t>DFG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>GB9720910936583000000000</t>
-  </si>
-  <si>
-    <t>GMG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DE9301821135910205540000</t>
-  </si>
-  <si>
-    <t>MLG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DE7822631245526916432102</t>
-  </si>
-  <si>
-    <t>IAG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES2120960043043075700000</t>
-  </si>
-  <si>
-    <t>IAG01@Agua2024.com</t>
-  </si>
-  <si>
-    <t>SM7325635478321002541225</t>
-  </si>
-  <si>
-    <t>GPG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES6832154697195423121000</t>
-  </si>
-  <si>
-    <t>RGG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>GB5520008521528775113366</t>
-  </si>
-  <si>
-    <t>AFG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES8020960043033000100000</t>
-  </si>
-  <si>
-    <t>APM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>GB0836585214290025478551</t>
-  </si>
-  <si>
-    <t>GMM03@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9012548523465214585214</t>
-  </si>
-  <si>
-    <t>ALM01@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES6931624561042546920007</t>
-  </si>
-  <si>
-    <t>LDM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES1436154231712500312566</t>
-  </si>
-  <si>
-    <t>AD00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES8244875664127231645789</t>
-  </si>
-  <si>
-    <t>LR00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES1633620012937852100256</t>
-  </si>
-  <si>
-    <t>SBG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES1933218885441445121022</t>
-  </si>
-  <si>
-    <t>AFG01@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES8462581542713690044508</t>
-  </si>
-  <si>
-    <t>DGG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES3925165151118666365100</t>
-  </si>
-  <si>
-    <t>ROG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>SOG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>PT3536952365020014425254</t>
-  </si>
-  <si>
-    <t>VVG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9565168874641561561500</t>
-  </si>
-  <si>
-    <t>VMG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES3220960583831234500000</t>
-  </si>
-  <si>
-    <t>MBG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7221416325811510005514</t>
-  </si>
-  <si>
-    <t>CBG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>LU0932628484504115151115</t>
-  </si>
-  <si>
-    <t>MSH00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES8163516541828944000984</t>
-  </si>
-  <si>
-    <t>SDM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>23658965274585223202</t>
-  </si>
-  <si>
-    <t>ES6223658965274585223202</t>
-  </si>
-  <si>
-    <t>EGM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>FI6132658012367712548745</t>
-  </si>
-  <si>
-    <t>GPM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7223652365142254222000</t>
-  </si>
-  <si>
-    <t>EAM00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9232584216971684051000</t>
-  </si>
-  <si>
-    <t>MG00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>LT9321856333126985542360</t>
-  </si>
-  <si>
-    <t>BDC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES5736245978133245679001</t>
-  </si>
-  <si>
-    <t>NGC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7631245164156597845124</t>
-  </si>
-  <si>
-    <t>MLC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>SM4423221158252545471411</t>
-  </si>
-  <si>
-    <t>MH00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>SE6832574512085411002255</t>
-  </si>
-  <si>
-    <t>MLC01@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES4420960043013468900000</t>
-  </si>
-  <si>
-    <t>CFC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES5631215643855060225021</t>
-  </si>
-  <si>
-    <t>CGC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES1665165654918886005001</t>
-  </si>
-  <si>
-    <t>KSC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>65645150865168448896</t>
-  </si>
-  <si>
-    <t>AT8365645150865168448896</t>
-  </si>
-  <si>
-    <t>MHC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>26551681807651415636</t>
-  </si>
-  <si>
-    <t>IT3526551681807651415636</t>
-  </si>
-  <si>
-    <t>CLD00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>HU2399558741836555551120</t>
-  </si>
-  <si>
-    <t>MFD00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>51556584221251000254</t>
-  </si>
-  <si>
-    <t>IE6851556584221251000254</t>
-  </si>
-  <si>
-    <t>GMM04@Agua2024.com</t>
-  </si>
-  <si>
-    <t>DK9032541112811220000588</t>
-  </si>
-  <si>
-    <t>IVC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>62541122421110105611</t>
-  </si>
-  <si>
-    <t>LT9362541122421110105611</t>
-  </si>
-  <si>
-    <t>DMC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES6855065688761051056105</t>
-  </si>
-  <si>
-    <t>EBC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES7426221011628048788896</t>
-  </si>
-  <si>
-    <t>NBC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9712548521518742146695</t>
-  </si>
-  <si>
-    <t>MSC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9001826530120201560000</t>
-  </si>
-  <si>
-    <t>MDC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES9021651651812511133551</t>
-  </si>
-  <si>
-    <t>MFC00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>ES6851651487910005118185</t>
-  </si>
-  <si>
-    <t>CDD00@Agua2024.com</t>
-  </si>
-  <si>
-    <t>AT3122515651915640081000</t>
-  </si>
-  <si>
-    <t>HPD00@Agua2024.com</t>
   </si>
 </sst>
 </file>
@@ -2564,12 +2015,6 @@
       <c r="H2" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="I2" t="s" s="0">
-        <v>504</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>505</v>
-      </c>
       <c r="K2" t="s" s="0">
         <v>264</v>
       </c>
@@ -2614,12 +2059,6 @@
       <c r="H3" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="I3" t="s" s="0">
-        <v>506</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>507</v>
-      </c>
       <c r="K3" t="s" s="0">
         <v>264</v>
       </c>
@@ -2664,12 +2103,6 @@
       <c r="H4" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="I4" t="s" s="0">
-        <v>508</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>509</v>
-      </c>
       <c r="K4" t="s" s="0">
         <v>264</v>
       </c>
@@ -2714,12 +2147,6 @@
       <c r="H5" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="I5" t="s" s="0">
-        <v>510</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>511</v>
-      </c>
       <c r="K5" t="s" s="0">
         <v>264</v>
       </c>
@@ -2764,12 +2191,6 @@
       <c r="H6" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="I6" t="s" s="0">
-        <v>512</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>513</v>
-      </c>
       <c r="K6" t="s" s="0">
         <v>264</v>
       </c>
@@ -2814,12 +2235,6 @@
       <c r="H7" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="I7" t="s" s="0">
-        <v>514</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>515</v>
-      </c>
       <c r="K7" t="s" s="0">
         <v>264</v>
       </c>
@@ -2864,12 +2279,6 @@
       <c r="H8" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="I8" t="s" s="0">
-        <v>516</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>517</v>
-      </c>
       <c r="K8" t="s" s="0">
         <v>264</v>
       </c>
@@ -2914,12 +2323,6 @@
       <c r="H9" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="I9" t="s" s="0">
-        <v>518</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>519</v>
-      </c>
       <c r="K9" t="s" s="0">
         <v>264</v>
       </c>
@@ -2964,12 +2367,6 @@
       <c r="H10" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="I10" t="s" s="0">
-        <v>520</v>
-      </c>
-      <c r="J10" t="s" s="0">
-        <v>521</v>
-      </c>
       <c r="K10" t="s" s="0">
         <v>264</v>
       </c>
@@ -3014,12 +2411,6 @@
       <c r="H11" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="I11" t="s" s="0">
-        <v>522</v>
-      </c>
-      <c r="J11" t="s" s="0">
-        <v>523</v>
-      </c>
       <c r="K11" t="s" s="0">
         <v>264</v>
       </c>
@@ -3064,12 +2455,6 @@
       <c r="H12" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="I12" t="s" s="0">
-        <v>524</v>
-      </c>
-      <c r="J12" t="s" s="0">
-        <v>525</v>
-      </c>
       <c r="K12" t="s" s="0">
         <v>264</v>
       </c>
@@ -3113,12 +2498,6 @@
       </c>
       <c r="H13" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="I13" t="s" s="0">
-        <v>526</v>
-      </c>
-      <c r="J13" t="s" s="0">
-        <v>527</v>
       </c>
       <c r="K13" t="s" s="0">
         <v>264</v>
@@ -3214,12 +2593,6 @@
       <c r="H16" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="I16" t="s" s="0">
-        <v>528</v>
-      </c>
-      <c r="J16" t="s" s="0">
-        <v>529</v>
-      </c>
       <c r="K16" t="s" s="0">
         <v>264</v>
       </c>
@@ -3264,12 +2637,6 @@
       <c r="H17" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="I17" t="s" s="0">
-        <v>530</v>
-      </c>
-      <c r="J17" t="s" s="0">
-        <v>531</v>
-      </c>
       <c r="K17" t="s" s="0">
         <v>264</v>
       </c>
@@ -3300,7 +2667,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>503</v>
+        <v>188</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -3313,12 +2680,6 @@
       </c>
       <c r="H18" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="I18" t="s" s="0">
-        <v>532</v>
-      </c>
-      <c r="J18" t="s" s="0">
-        <v>533</v>
       </c>
       <c r="K18" t="s" s="0">
         <v>264</v>
@@ -3364,12 +2725,6 @@
       <c r="H19" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="I19" t="s" s="0">
-        <v>534</v>
-      </c>
-      <c r="J19" t="s" s="0">
-        <v>535</v>
-      </c>
       <c r="K19" t="s" s="0">
         <v>264</v>
       </c>
@@ -3400,7 +2755,7 @@
         <v>145</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>392</v>
@@ -3413,12 +2768,6 @@
       </c>
       <c r="H20" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="I20" t="s" s="0">
-        <v>536</v>
-      </c>
-      <c r="J20" t="s" s="0">
-        <v>537</v>
       </c>
       <c r="K20" t="s" s="0">
         <v>264</v>
@@ -3464,12 +2813,6 @@
       <c r="H21" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="I21" t="s" s="0">
-        <v>538</v>
-      </c>
-      <c r="J21" t="s" s="0">
-        <v>539</v>
-      </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
       </c>
@@ -3511,12 +2854,6 @@
       <c r="H22" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="I22" t="s" s="0">
-        <v>540</v>
-      </c>
-      <c r="J22" t="s" s="0">
-        <v>541</v>
-      </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
       </c>
@@ -3558,12 +2895,6 @@
       <c r="H23" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="I23" t="s" s="0">
-        <v>542</v>
-      </c>
-      <c r="J23" t="s" s="0">
-        <v>543</v>
-      </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
       </c>
@@ -3605,12 +2936,6 @@
       <c r="H24" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="I24" t="s" s="0">
-        <v>544</v>
-      </c>
-      <c r="J24" t="s" s="0">
-        <v>545</v>
-      </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
       </c>
@@ -3651,12 +2976,6 @@
       </c>
       <c r="H25" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="I25" t="s" s="0">
-        <v>546</v>
-      </c>
-      <c r="J25" t="s" s="0">
-        <v>547</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
@@ -3710,12 +3029,6 @@
       <c r="H27" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="I27" t="s" s="0">
-        <v>548</v>
-      </c>
-      <c r="J27" t="s" s="0">
-        <v>549</v>
-      </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
       </c>
@@ -3760,12 +3073,6 @@
       <c r="H28" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="I28" t="s" s="0">
-        <v>550</v>
-      </c>
-      <c r="J28" t="s" s="0">
-        <v>551</v>
-      </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
       </c>
@@ -3810,12 +3117,6 @@
       <c r="H29" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="I29" t="s" s="0">
-        <v>552</v>
-      </c>
-      <c r="J29" t="s" s="0">
-        <v>553</v>
-      </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
       </c>
@@ -3860,12 +3161,6 @@
       <c r="H30" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="I30" t="s" s="0">
-        <v>554</v>
-      </c>
-      <c r="J30" t="s" s="0">
-        <v>555</v>
-      </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
       </c>
@@ -3910,12 +3205,6 @@
       <c r="H31" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="I31" t="s" s="0">
-        <v>556</v>
-      </c>
-      <c r="J31" t="s" s="0">
-        <v>557</v>
-      </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
       </c>
@@ -3959,12 +3248,6 @@
       </c>
       <c r="H32" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="I32" t="s" s="0">
-        <v>558</v>
-      </c>
-      <c r="J32" t="s" s="0">
-        <v>559</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -4028,12 +3311,6 @@
       <c r="H36" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I36" t="s" s="0">
-        <v>560</v>
-      </c>
-      <c r="J36" t="s" s="0">
-        <v>561</v>
-      </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
       </c>
@@ -4078,12 +3355,6 @@
       <c r="H37" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="I37" t="s" s="0">
-        <v>562</v>
-      </c>
-      <c r="J37" t="s" s="0">
-        <v>563</v>
-      </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
       </c>
@@ -4114,7 +3385,7 @@
         <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>394</v>
@@ -4127,12 +3398,6 @@
       </c>
       <c r="H38" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="I38" t="s" s="0">
-        <v>564</v>
-      </c>
-      <c r="J38" t="s" s="0">
-        <v>565</v>
       </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
@@ -4178,12 +3443,6 @@
       <c r="H39" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="I39" t="s" s="0">
-        <v>566</v>
-      </c>
-      <c r="J39" t="s" s="0">
-        <v>567</v>
-      </c>
       <c r="K39" t="s" s="0">
         <v>264</v>
       </c>
@@ -4228,12 +3487,6 @@
       <c r="H40" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="I40" t="s" s="0">
-        <v>568</v>
-      </c>
-      <c r="J40" t="s" s="0">
-        <v>569</v>
-      </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
       </c>
@@ -4278,12 +3531,6 @@
       <c r="H41" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="I41" t="s" s="0">
-        <v>570</v>
-      </c>
-      <c r="J41" t="s" s="0">
-        <v>571</v>
-      </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
       </c>
@@ -4314,7 +3561,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>397</v>
@@ -4327,12 +3574,6 @@
       </c>
       <c r="H42" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="I42" t="s" s="0">
-        <v>572</v>
-      </c>
-      <c r="J42" t="s" s="0">
-        <v>573</v>
       </c>
       <c r="K42" t="s" s="0">
         <v>264</v>
@@ -4378,12 +3619,6 @@
       <c r="H43" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="I43" t="s" s="0">
-        <v>574</v>
-      </c>
-      <c r="J43" t="s" s="0">
-        <v>575</v>
-      </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
       </c>
@@ -4428,12 +3663,6 @@
       <c r="H44" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I44" t="s" s="0">
-        <v>576</v>
-      </c>
-      <c r="J44" t="s" s="0">
-        <v>577</v>
-      </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
       </c>
@@ -4478,12 +3707,6 @@
       <c r="H45" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="I45" t="s" s="0">
-        <v>578</v>
-      </c>
-      <c r="J45" t="s" s="0">
-        <v>579</v>
-      </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
       </c>
@@ -4528,12 +3751,6 @@
       <c r="H46" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="I46" t="s" s="0">
-        <v>580</v>
-      </c>
-      <c r="J46" t="s" s="0">
-        <v>581</v>
-      </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
       </c>
@@ -4578,12 +3795,6 @@
       <c r="H47" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="I47" t="s" s="0">
-        <v>582</v>
-      </c>
-      <c r="J47" t="s" s="0">
-        <v>583</v>
-      </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
       </c>
@@ -4628,12 +3839,6 @@
       <c r="H48" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="I48" t="s" s="0">
-        <v>584</v>
-      </c>
-      <c r="J48" t="s" s="0">
-        <v>585</v>
-      </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
       </c>
@@ -4678,12 +3883,6 @@
       <c r="H49" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="I49" t="s" s="0">
-        <v>586</v>
-      </c>
-      <c r="J49" t="s" s="0">
-        <v>587</v>
-      </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
       </c>
@@ -4728,12 +3927,6 @@
       <c r="H50" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="I50" t="s" s="0">
-        <v>588</v>
-      </c>
-      <c r="J50" t="s" s="0">
-        <v>589</v>
-      </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
       </c>
@@ -4778,12 +3971,6 @@
       <c r="H51" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="I51" t="s" s="0">
-        <v>590</v>
-      </c>
-      <c r="J51" t="s" s="0">
-        <v>591</v>
-      </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
       </c>
@@ -4828,12 +4015,6 @@
       <c r="H52" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="I52" t="s" s="0">
-        <v>592</v>
-      </c>
-      <c r="J52" t="s" s="0">
-        <v>593</v>
-      </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
       </c>
@@ -4878,12 +4059,6 @@
       <c r="H53" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I53" t="s" s="0">
-        <v>594</v>
-      </c>
-      <c r="J53" t="s" s="0">
-        <v>595</v>
-      </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
       </c>
@@ -4971,12 +4146,6 @@
       </c>
       <c r="H55" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="I55" t="s" s="0">
-        <v>596</v>
-      </c>
-      <c r="J55" t="s" s="0">
-        <v>597</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -5046,12 +4215,6 @@
       <c r="H60" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="I60" t="s" s="0">
-        <v>598</v>
-      </c>
-      <c r="J60" t="s" s="0">
-        <v>599</v>
-      </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
       </c>
@@ -5096,12 +4259,6 @@
       <c r="H61" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="I61" t="s" s="0">
-        <v>600</v>
-      </c>
-      <c r="J61" t="s" s="0">
-        <v>601</v>
-      </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
       </c>
@@ -5146,12 +4303,6 @@
       <c r="H62" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="I62" t="s" s="0">
-        <v>602</v>
-      </c>
-      <c r="J62" t="s" s="0">
-        <v>603</v>
-      </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
       </c>
@@ -5196,12 +4347,6 @@
       <c r="H63" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="I63" t="s" s="0">
-        <v>604</v>
-      </c>
-      <c r="J63" t="s" s="0">
-        <v>605</v>
-      </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
       </c>
@@ -5243,12 +4388,6 @@
       <c r="H64" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="I64" t="s" s="0">
-        <v>606</v>
-      </c>
-      <c r="J64" t="s" s="0">
-        <v>607</v>
-      </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
       </c>
@@ -5290,12 +4429,6 @@
       <c r="H65" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="I65" t="s" s="0">
-        <v>608</v>
-      </c>
-      <c r="J65" t="s" s="0">
-        <v>609</v>
-      </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
       </c>
@@ -5367,7 +4500,7 @@
         <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>405</v>
@@ -5380,12 +4513,6 @@
       </c>
       <c r="H67" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="I67" t="s" s="0">
-        <v>610</v>
-      </c>
-      <c r="J67" t="s" s="0">
-        <v>611</v>
       </c>
       <c r="K67" t="s" s="0">
         <v>264</v>
@@ -5431,12 +4558,6 @@
       <c r="H68" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="I68" t="s" s="0">
-        <v>612</v>
-      </c>
-      <c r="J68" t="s" s="0">
-        <v>613</v>
-      </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
       </c>
@@ -5481,12 +4602,6 @@
       <c r="H69" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="I69" t="s" s="0">
-        <v>614</v>
-      </c>
-      <c r="J69" t="s" s="0">
-        <v>615</v>
-      </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
       </c>
@@ -5531,12 +4646,6 @@
       <c r="H70" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="I70" t="s" s="0">
-        <v>616</v>
-      </c>
-      <c r="J70" t="s" s="0">
-        <v>617</v>
-      </c>
       <c r="K70" t="s" s="0">
         <v>264</v>
       </c>
@@ -5581,12 +4690,6 @@
       <c r="H71" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="I71" t="s" s="0">
-        <v>598</v>
-      </c>
-      <c r="J71" t="s" s="0">
-        <v>618</v>
-      </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
       </c>
@@ -5631,12 +4734,6 @@
       <c r="H72" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="I72" t="s" s="0">
-        <v>619</v>
-      </c>
-      <c r="J72" t="s" s="0">
-        <v>620</v>
-      </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
       </c>
@@ -5681,12 +4778,6 @@
       <c r="H73" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="I73" t="s" s="0">
-        <v>621</v>
-      </c>
-      <c r="J73" t="s" s="0">
-        <v>622</v>
-      </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
       </c>
@@ -5731,12 +4822,6 @@
       <c r="H74" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="I74" t="s" s="0">
-        <v>623</v>
-      </c>
-      <c r="J74" t="s" s="0">
-        <v>624</v>
-      </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
       </c>
@@ -5781,12 +4866,6 @@
       <c r="H75" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I75" t="s" s="0">
-        <v>625</v>
-      </c>
-      <c r="J75" t="s" s="0">
-        <v>626</v>
-      </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
       </c>
@@ -5830,12 +4909,6 @@
       </c>
       <c r="H76" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="I76" t="s" s="0">
-        <v>627</v>
-      </c>
-      <c r="J76" t="s" s="0">
-        <v>628</v>
       </c>
       <c r="K76" t="s" s="0">
         <v>264</v>
@@ -5931,12 +5004,6 @@
       <c r="H79" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="I79" t="s" s="0">
-        <v>629</v>
-      </c>
-      <c r="J79" t="s" s="0">
-        <v>630</v>
-      </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
       </c>
@@ -5979,13 +5046,7 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="I80" t="s" s="0">
-        <v>632</v>
-      </c>
-      <c r="J80" t="s" s="0">
-        <v>633</v>
+        <v>332</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
@@ -6031,12 +5092,6 @@
       <c r="H81" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="I81" t="s" s="0">
-        <v>634</v>
-      </c>
-      <c r="J81" t="s" s="0">
-        <v>635</v>
-      </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
       </c>
@@ -6081,12 +5136,6 @@
       <c r="H82" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="I82" t="s" s="0">
-        <v>636</v>
-      </c>
-      <c r="J82" t="s" s="0">
-        <v>637</v>
-      </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
       </c>
@@ -6171,12 +5220,6 @@
       </c>
       <c r="H84" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="I84" t="s" s="0">
-        <v>638</v>
-      </c>
-      <c r="J84" t="s" s="0">
-        <v>639</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -6272,12 +5315,6 @@
       <c r="H87" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="I87" t="s" s="0">
-        <v>640</v>
-      </c>
-      <c r="J87" t="s" s="0">
-        <v>641</v>
-      </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
       </c>
@@ -6322,12 +5359,6 @@
       <c r="H88" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I88" t="s" s="0">
-        <v>642</v>
-      </c>
-      <c r="J88" t="s" s="0">
-        <v>643</v>
-      </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
       </c>
@@ -6372,12 +5403,6 @@
       <c r="H89" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="I89" t="s" s="0">
-        <v>644</v>
-      </c>
-      <c r="J89" t="s" s="0">
-        <v>645</v>
-      </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
       </c>
@@ -6419,12 +5444,6 @@
       <c r="H90" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="I90" t="s" s="0">
-        <v>646</v>
-      </c>
-      <c r="J90" t="s" s="0">
-        <v>647</v>
-      </c>
       <c r="K90" t="s" s="0">
         <v>264</v>
       </c>
@@ -6469,12 +5488,6 @@
       <c r="H91" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="I91" t="s" s="0">
-        <v>648</v>
-      </c>
-      <c r="J91" t="s" s="0">
-        <v>649</v>
-      </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
       </c>
@@ -6519,12 +5532,6 @@
       <c r="H92" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="I92" t="s" s="0">
-        <v>650</v>
-      </c>
-      <c r="J92" t="s" s="0">
-        <v>651</v>
-      </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
       </c>
@@ -6569,12 +5576,6 @@
       <c r="H93" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="I93" t="s" s="0">
-        <v>652</v>
-      </c>
-      <c r="J93" t="s" s="0">
-        <v>653</v>
-      </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
       </c>
@@ -6660,12 +5661,6 @@
       </c>
       <c r="H95" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="I95" t="s" s="0">
-        <v>654</v>
-      </c>
-      <c r="J95" t="s" s="0">
-        <v>655</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -6745,13 +5740,7 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="I102" t="s" s="0">
-        <v>657</v>
-      </c>
-      <c r="J102" t="s" s="0">
-        <v>658</v>
+        <v>347</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -6795,13 +5784,7 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="I103" t="s" s="0">
-        <v>660</v>
-      </c>
-      <c r="J103" t="s" s="0">
-        <v>661</v>
+        <v>348</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
@@ -6847,12 +5830,6 @@
       <c r="H104" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="I104" t="s" s="0">
-        <v>662</v>
-      </c>
-      <c r="J104" t="s" s="0">
-        <v>663</v>
-      </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
       </c>
@@ -6939,13 +5916,7 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="I106" t="s" s="0">
-        <v>665</v>
-      </c>
-      <c r="J106" t="s" s="0">
-        <v>666</v>
+        <v>351</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
@@ -7111,12 +6082,6 @@
       <c r="H127" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="I127" t="s" s="0">
-        <v>667</v>
-      </c>
-      <c r="J127" t="s" s="0">
-        <v>668</v>
-      </c>
       <c r="K127" t="s" s="0">
         <v>264</v>
       </c>
@@ -7159,13 +6124,7 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="I128" t="s" s="0">
-        <v>670</v>
-      </c>
-      <c r="J128" t="s" s="0">
-        <v>671</v>
+        <v>353</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -7211,12 +6170,6 @@
       <c r="H129" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I129" t="s" s="0">
-        <v>672</v>
-      </c>
-      <c r="J129" t="s" s="0">
-        <v>673</v>
-      </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
       </c>
@@ -7261,12 +6214,6 @@
       <c r="H130" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="I130" t="s" s="0">
-        <v>674</v>
-      </c>
-      <c r="J130" t="s" s="0">
-        <v>675</v>
-      </c>
       <c r="K130" t="s" s="0">
         <v>264</v>
       </c>
@@ -7311,12 +6258,6 @@
       <c r="H131" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="I131" t="s" s="0">
-        <v>676</v>
-      </c>
-      <c r="J131" t="s" s="0">
-        <v>677</v>
-      </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
       </c>
@@ -7361,12 +6302,6 @@
       <c r="H132" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="I132" t="s" s="0">
-        <v>678</v>
-      </c>
-      <c r="J132" t="s" s="0">
-        <v>679</v>
-      </c>
       <c r="K132" t="s" s="0">
         <v>264</v>
       </c>
@@ -7411,12 +6346,6 @@
       <c r="H133" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="I133" t="s" s="0">
-        <v>680</v>
-      </c>
-      <c r="J133" t="s" s="0">
-        <v>681</v>
-      </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
       </c>
@@ -7461,12 +6390,6 @@
       <c r="H134" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="I134" t="s" s="0">
-        <v>682</v>
-      </c>
-      <c r="J134" t="s" s="0">
-        <v>683</v>
-      </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
       </c>
@@ -7552,12 +6475,6 @@
       </c>
       <c r="H136" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="I136" t="s" s="0">
-        <v>684</v>
-      </c>
-      <c r="J136" t="s" s="0">
-        <v>685</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>

</xml_diff>